<commit_message>
set it up so it actually run saveCSVs and 4thpass
</commit_message>
<xml_diff>
--- a/predictor effect plots.xlsx
+++ b/predictor effect plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\CSUF\ISDS577\projects\Capstone-577\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B003577B-F93D-452A-8C5F-D7A018ECA82C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A518E7-1FCF-4894-B713-58363F8983B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7995" yWindow="3060" windowWidth="19560" windowHeight="14010" xr2:uid="{9619FFE6-B5E3-4413-AA5D-8F223E55038A}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="19845" windowHeight="13740" xr2:uid="{9619FFE6-B5E3-4413-AA5D-8F223E55038A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>V8512</t>
   </si>
@@ -106,13 +106,49 @@
   </si>
   <si>
     <t>X5</t>
+  </si>
+  <si>
+    <t>V8505</t>
+  </si>
+  <si>
+    <t>V8536</t>
+  </si>
+  <si>
+    <t>Min.</t>
+  </si>
+  <si>
+    <t>Max.</t>
+  </si>
+  <si>
+    <t>V7118</t>
+  </si>
+  <si>
+    <t>V8514</t>
+  </si>
+  <si>
+    <t>1st Qu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median </t>
+  </si>
+  <si>
+    <t>3rd Qu.</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>stdev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +161,11 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,11 +188,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,7 +251,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Effect Plots</a:t>
+              <a:t> Effect Plots of response term based on fixed means of other predictor terms</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1244,16 +1287,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1283,7 +1326,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9839325" y="66675"/>
+          <a:off x="314325" y="57150"/>
           <a:ext cx="5943600" cy="1171575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1305,16 +1348,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1337,6 +1380,67 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="https://lh3.googleusercontent.com/0gDOHgmtApe-XU9cu7gZWmXFAHbA5RhBG2kW22YgpBCDXHgdv4_WVwr8vpLUFAAlgQUUqoSvxA4O25oBZfm7vaZL-CdYBq1NOrOp-WG2xNgJViUptlnVRGGjSW73KN7OAMldR6c">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D207AA-458C-4008-8222-7E9F53D238B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6705600" y="0"/>
+          <a:ext cx="4486275" cy="1657350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1639,15 +1743,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC55E4CF-1AE4-48CC-A3CA-AD3D5F053292}">
-  <dimension ref="A8:U14"/>
+  <dimension ref="A8:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="D8">
         <v>1</v>
       </c>
@@ -1664,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -1681,7 +1785,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -1722,7 +1826,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1778,7 +1882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1827,27 +1931,27 @@
         <v>1</v>
       </c>
       <c r="Q12">
-        <f>EXP(J12)/(1+EXP(J12))</f>
+        <f t="shared" ref="Q12:U13" si="0">EXP(J12)/(1+EXP(J12))</f>
         <v>0.61891714621206517</v>
       </c>
       <c r="R12">
-        <f>EXP(K12)/(1+EXP(K12))</f>
+        <f t="shared" si="0"/>
         <v>0.59980759004791806</v>
       </c>
       <c r="S12">
-        <f>EXP(L12)/(1+EXP(L12))</f>
+        <f t="shared" si="0"/>
         <v>0.68691131960741614</v>
       </c>
       <c r="T12">
-        <f>EXP(M12)/(1+EXP(M12))</f>
+        <f t="shared" si="0"/>
         <v>0.39256728399772595</v>
       </c>
       <c r="U12">
-        <f>EXP(N12)/(1+EXP(N12))</f>
+        <f t="shared" si="0"/>
         <v>0.53962575251621003</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="I13">
         <v>0</v>
       </c>
@@ -1875,27 +1979,27 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>EXP(J13)/(1+EXP(J13))</f>
+        <f t="shared" si="0"/>
         <v>0.48564259733785148</v>
       </c>
       <c r="R13">
-        <f>EXP(K13)/(1+EXP(K13))</f>
+        <f t="shared" si="0"/>
         <v>0.47560774433741054</v>
       </c>
       <c r="S13">
-        <f>EXP(L13)/(1+EXP(L13))</f>
+        <f t="shared" si="0"/>
         <v>0.48241693495454535</v>
       </c>
       <c r="T13">
-        <f>EXP(M13)/(1+EXP(M13))</f>
+        <f t="shared" si="0"/>
         <v>0.52202237600398393</v>
       </c>
       <c r="U13">
-        <f>EXP(N13)/(1+EXP(N13))</f>
+        <f t="shared" si="0"/>
         <v>0.47733207631954067</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -1913,10 +2017,277 @@
       </c>
       <c r="H14" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4980</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>0.12989999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.2203</v>
+      </c>
+      <c r="F21">
+        <v>9.7390000000000004E-2</v>
+      </c>
+      <c r="G21">
+        <v>0.25</v>
+      </c>
+      <c r="H21">
+        <v>0.14319999999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.22889999999999999</v>
+      </c>
+      <c r="J21">
+        <v>0.41570000000000001</v>
+      </c>
+      <c r="K21">
+        <v>2.0480000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0.25</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="3">
+        <f>SQRT((D21*1-D21)/$D$16)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" ref="E26:K26" si="1">SQRT((E21*1-E21)/$D$16)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update predictor effect plots.xlsx
</commit_message>
<xml_diff>
--- a/predictor effect plots.xlsx
+++ b/predictor effect plots.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\CSUF\ISDS577\projects\Capstone-577\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D46542-88BD-48D6-8737-F9689640CFA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B46FD3-ADC4-4C98-B5A9-3701267A66E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9619FFE6-B5E3-4413-AA5D-8F223E55038A}"/>
   </bookViews>
   <sheets>
-    <sheet name="V7118 - PSYD LIFETIME" sheetId="1" r:id="rId1"/>
+    <sheet name="V7118 - PSYD LIFETIME - e 35%" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -343,7 +343,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$R$2</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$R$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -366,7 +366,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$R$3:$R$4</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$R$3:$R$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -391,7 +391,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$S$2</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$S$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -414,7 +414,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$S$3:$S$4</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$S$3:$S$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -439,7 +439,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$T$2</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$T$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -462,7 +462,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$T$3:$T$4</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$T$3:$T$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -487,7 +487,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$U$2</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$U$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -510,7 +510,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$U$3:$U$4</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$U$3:$U$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -535,7 +535,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$V$2</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$V$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -558,7 +558,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$V$3:$V$4</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$V$3:$V$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -864,7 +864,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$R$6:$V$6</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$R$6:$V$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -887,7 +887,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'V7118 - PSYD LIFETIME'!$R$7:$V$7</c:f>
+              <c:f>'V7118 - PSYD LIFETIME - e 35%'!$R$7:$V$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2438,16 +2438,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2477,8 +2477,69 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1228724" y="5229225"/>
+          <a:off x="14973299" y="4581525"/>
           <a:ext cx="2905125" cy="2905125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C96E7E80-FEB4-4972-82DC-0E305A8352AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3105150" cy="3105150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2800,7 +2861,7 @@
   <dimension ref="A2:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
way better rmse handling with optimal values for both population and monte carlo model in saveCSVs.R
</commit_message>
<xml_diff>
--- a/predictor effect plots.xlsx
+++ b/predictor effect plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\CSUF\ISDS577\projects\Capstone-577\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B46FD3-ADC4-4C98-B5A9-3701267A66E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151E8593-2E55-4418-9876-46C45FEE06A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9619FFE6-B5E3-4413-AA5D-8F223E55038A}"/>
   </bookViews>
@@ -19,6 +19,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -303,6 +308,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10943842959372539"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2245,15 +2258,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2342,15 +2355,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>109535</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>319085</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2377,23 +2390,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBEF509A-F6E0-4425-87A8-D851EE44D435}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E65818A3-EDEF-4630-A69B-3EF8BAAE90C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2416,130 +2429,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1228725" y="2324100"/>
-          <a:ext cx="2943225" cy="2943225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E65818A3-EDEF-4630-A69B-3EF8BAAE90C6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14973299" y="4581525"/>
+          <a:off x="14963774" y="4371975"/>
           <a:ext cx="2905125" cy="2905125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C96E7E80-FEB4-4972-82DC-0E305A8352AE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="3105150" cy="3105150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2858,10 +2749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC55E4CF-1AE4-48CC-A3CA-AD3D5F053292}">
-  <dimension ref="A2:Z36"/>
+  <dimension ref="A2:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H16" sqref="H16:M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2888,23 +2779,23 @@
         <v>1</v>
       </c>
       <c r="R3">
-        <f>EXP(J12)/(1+EXP(J12))</f>
+        <f t="shared" ref="R3:V4" si="0">EXP(J12)/(1+EXP(J12))</f>
         <v>0.6091059884508675</v>
       </c>
       <c r="S3">
-        <f>EXP(K12)/(1+EXP(K12))</f>
+        <f t="shared" si="0"/>
         <v>0.64354891356190846</v>
       </c>
       <c r="T3">
-        <f>EXP(L12)/(1+EXP(L12))</f>
+        <f t="shared" si="0"/>
         <v>0.77145248431830904</v>
       </c>
       <c r="U3">
-        <f>EXP(M12)/(1+EXP(M12))</f>
+        <f t="shared" si="0"/>
         <v>0.41117293904524327</v>
       </c>
       <c r="V3">
-        <f>EXP(N12)/(1+EXP(N12))</f>
+        <f t="shared" si="0"/>
         <v>0.67407761195273008</v>
       </c>
     </row>
@@ -2913,23 +2804,23 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <f>EXP(J13)/(1+EXP(J13))</f>
+        <f t="shared" si="0"/>
         <v>0.49017772289274664</v>
       </c>
       <c r="S4">
-        <f>EXP(K13)/(1+EXP(K13))</f>
+        <f t="shared" si="0"/>
         <v>0.47136661523360135</v>
       </c>
       <c r="T4">
-        <f>EXP(L13)/(1+EXP(L13))</f>
+        <f t="shared" si="0"/>
         <v>0.4408189505215595</v>
       </c>
       <c r="U4">
-        <f>EXP(M13)/(1+EXP(M13))</f>
+        <f t="shared" si="0"/>
         <v>0.51973758222053579</v>
       </c>
       <c r="V4">
-        <f>EXP(N13)/(1+EXP(N13))</f>
+        <f t="shared" si="0"/>
         <v>0.48748410909433987</v>
       </c>
     </row>
@@ -3181,7 +3072,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:22">
       <c r="H17" s="3" t="s">
         <v>18</v>
       </c>
@@ -3189,13 +3080,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:26">
+    <row r="18" spans="2:22">
       <c r="H18" s="3"/>
       <c r="O18" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:22">
       <c r="H19" s="3" t="s">
         <v>19</v>
       </c>
@@ -3203,7 +3094,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:22">
       <c r="H20" s="3" t="s">
         <v>20</v>
       </c>
@@ -3211,7 +3102,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:22">
       <c r="H21" s="3" t="s">
         <v>21</v>
       </c>
@@ -3219,7 +3110,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:26">
+    <row r="22" spans="2:22">
       <c r="H22" s="3" t="s">
         <v>22</v>
       </c>
@@ -3227,29 +3118,29 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:22">
       <c r="H23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="O23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Y23" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="2:26">
+    </row>
+    <row r="24" spans="2:22">
       <c r="H24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="2:26">
+      <c r="U24" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22">
       <c r="H25" s="3" t="s">
         <v>25</v>
       </c>
@@ -3257,7 +3148,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:26">
+    <row r="26" spans="2:22">
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -3272,7 +3163,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:22">
       <c r="H27" s="3" t="s">
         <v>27</v>
       </c>
@@ -3280,7 +3171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:22">
       <c r="H28" s="3" t="s">
         <v>28</v>
       </c>
@@ -3288,7 +3179,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:22">
       <c r="B29" t="s">
         <v>49</v>
       </c>
@@ -3297,7 +3188,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:26">
+    <row r="30" spans="2:22">
       <c r="H30" s="3" t="s">
         <v>29</v>
       </c>
@@ -3305,10 +3196,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="2:26">
+    <row r="31" spans="2:22">
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="2:26">
+    <row r="32" spans="2:22">
       <c r="H32" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
mcAppPop gains and ROC
</commit_message>
<xml_diff>
--- a/predictor effect plots.xlsx
+++ b/predictor effect plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\CSUF\ISDS577\projects\Capstone-577\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151E8593-2E55-4418-9876-46C45FEE06A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A133AD-B261-44CF-AFE8-95DBE7DCCA4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9619FFE6-B5E3-4413-AA5D-8F223E55038A}"/>
+    <workbookView xWindow="1020" yWindow="540" windowWidth="25275" windowHeight="14565" xr2:uid="{9619FFE6-B5E3-4413-AA5D-8F223E55038A}"/>
   </bookViews>
   <sheets>
     <sheet name="V7118 - PSYD LIFETIME - e 35%" sheetId="1" r:id="rId1"/>

</xml_diff>